<commit_message>
Initial Glider Design v3.0
- Python
- Small tweaks to give more realistic result
</commit_message>
<xml_diff>
--- a/01_Initial_Glider_Design/results/Nausicaa_v_3_0/nausicaa_results.xlsx
+++ b/01_Initial_Glider_Design/results/Nausicaa_v_3_0/nausicaa_results.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.586677829662333</v>
+        <v>4.586677829652073</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.000000079984837</v>
+        <v>8.000000079969384</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>65.00000064980111</v>
+        <v>65.00000064970294</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.366201640701398</v>
+        <v>2.366201640692703</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1474724807717653</v>
+        <v>0.1302879996247762</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10.98899039384496</v>
+        <v>12.01608239753199</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9876252701062175</v>
+        <v>0.9032065732239588</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.03999998999370397</v>
+        <v>0.03999999003510714</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5101475987534781</v>
+        <v>0.3999999900893299</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01999999000151666</v>
+        <v>0.019999990001299</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46734.95394346571</v>
+        <v>47617.94750078177</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.2649777484154517</v>
+        <v>-0.1351272611301569</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.328261646907273</v>
+        <v>0.7187750035881874</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.863352958781579</v>
+        <v>1.572085127265426</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2.683099062315335</v>
+        <v>1.244446304013794</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1488368396628513</v>
+        <v>0.1516489098467315</v>
       </c>
     </row>
     <row r="19">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2773355655614735</v>
+        <v>0.2384049957360621</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.328261646907273</v>
+        <v>0.7187750035881874</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.2518222535968294</v>
+        <v>0.283687908460051</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.06295556339920734</v>
+        <v>0.07092197711501275</v>
       </c>
     </row>
     <row r="24">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01585361185164646</v>
+        <v>0.02011970735160956</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.328261646907273</v>
+        <v>0.7187750035881874</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1247493863506291</v>
+        <v>0.144420588295566</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.06237469317531454</v>
+        <v>0.07221029414778299</v>
       </c>
     </row>
     <row r="29">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.007781204697429259</v>
+        <v>0.01042865316181868</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10.59306181431991</v>
+        <v>-0.6788869189165445</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-4.105410643542815</v>
+        <v>5.901049369916801e-07</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.001590411386175785</v>
+        <v>1.379937337878626e-06</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3.651562188062312</v>
+        <v>3.164437083943233</v>
       </c>
     </row>
     <row r="35">
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2.04505273759086e-09</v>
+        <v>1.589021735948907e-09</v>
       </c>
     </row>
     <row r="40">
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.05027592234786796</v>
+        <v>0.03683269640263574</v>
       </c>
     </row>
     <row r="41">
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-6.365211525391369e-18</v>
+        <v>-1.795779200810796e-17</v>
       </c>
     </row>
     <row r="42">
@@ -939,7 +939,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.01393175183148838</v>
+        <v>0.006065873232640401</v>
       </c>
     </row>
     <row r="43">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0263962472067103</v>
+        <v>0.01648895843197087</v>
       </c>
     </row>
     <row r="44">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.01160005901615739</v>
+        <v>0.003226500725865624</v>
       </c>
     </row>
     <row r="45">
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.03792808307911333</v>
+        <v>0.01968929380950151</v>
       </c>
     </row>
     <row r="46">
@@ -979,7 +979,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-1.111338514328156e-20</v>
+        <v>7.54530294616237e-22</v>
       </c>
     </row>
     <row r="47">
@@ -989,7 +989,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-4.765117435489657e-05</v>
+        <v>-6.933513753893814e-05</v>
       </c>
     </row>
     <row r="48">
@@ -999,7 +999,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2.202503152166251e-20</v>
+        <v>2.410209944985826e-20</v>
       </c>
     </row>
     <row r="49">
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.08472660939497025</v>
+        <v>0.07420932212624523</v>
       </c>
     </row>
     <row r="50">
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.001805061077863655</v>
+        <v>0.002580667540697819</v>
       </c>
     </row>
     <row r="51">
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.0008777782761761291</v>
+        <v>0.001361936639877316</v>
       </c>
     </row>
     <row r="52">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.01433915455790452</v>
+        <v>0.007685120382465098</v>
       </c>
     </row>
     <row r="57">
@@ -1099,7 +1099,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-9.999724513271972e-09</v>
+        <v>-9.999677911335569e-09</v>
       </c>
     </row>
     <row r="59">
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.0109238874645752</v>
+        <v>0.009650962935168605</v>
       </c>
     </row>
     <row r="60">
@@ -1119,7 +1119,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.03720920991571283</v>
+        <v>-0.03791222746168288</v>
       </c>
     </row>
     <row r="61">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.03720920991571283</v>
+        <v>-0.03791222746168288</v>
       </c>
     </row>
     <row r="64">
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.9306551074579985</v>
+        <v>0.7858571652018056</v>
       </c>
     </row>
     <row r="65">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.04361345219490978</v>
+        <v>0.01707125488268932</v>
       </c>
     </row>
     <row r="66">
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1.265306083508065</v>
+        <v>0.6478530264731746</v>
       </c>
     </row>
     <row r="67">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1.265306083508065</v>
+        <v>0.6478530264731746</v>
       </c>
     </row>
     <row r="70">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.1259111267984147</v>
+        <v>0.1418439542300255</v>
       </c>
     </row>
     <row r="71">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1.265886953731958</v>
+        <v>0.6465647094404043</v>
       </c>
     </row>
     <row r="73">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1.265886953731958</v>
+        <v>0.6465647094404043</v>
       </c>
     </row>
     <row r="76">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1247493863506291</v>
+        <v>0.144420588295566</v>
       </c>
     </row>
     <row r="78">
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.1679369869015546</v>
+        <v>-0.1716630531957717</v>
       </c>
     </row>
     <row r="79">
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.02076975409479859</v>
+        <v>-6.526460340647266e-09</v>
       </c>
     </row>
     <row r="80">
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3.433235532066039</v>
+        <v>3.029898005867883</v>
       </c>
     </row>
     <row r="81">
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-0.2845491758456503</v>
+        <v>3.026881886503915e-08</v>
       </c>
     </row>
     <row r="82">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-7.325130085833464e-14</v>
+        <v>1.500590016828562e-15</v>
       </c>
     </row>
     <row r="83">
@@ -1349,7 +1349,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.03366781786149638</v>
+        <v>7.967749093537576e-10</v>
       </c>
     </row>
     <row r="84">
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.1679369869015546</v>
+        <v>0.1716630531957717</v>
       </c>
     </row>
     <row r="85">
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-0.3115114044134071</v>
+        <v>-0.251687865128</v>
       </c>
     </row>
     <row r="86">
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.2845491758456503</v>
+        <v>-3.026881886503915e-08</v>
       </c>
     </row>
     <row r="87">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.2864656174322798</v>
+        <v>-3.008513443069427e-08</v>
       </c>
     </row>
     <row r="88">
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>3.423195830672083</v>
+        <v>3.024302125836964</v>
       </c>
     </row>
     <row r="89">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.02076975409479859</v>
+        <v>-6.526460340647266e-09</v>
       </c>
     </row>
     <row r="90">
@@ -1419,7 +1419,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.3115114044134071</v>
+        <v>0.251687865128</v>
       </c>
     </row>
     <row r="91">
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.2845491758456503</v>
+        <v>-3.026881886503915e-08</v>
       </c>
     </row>
     <row r="92">
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-7.325130085833464e-14</v>
+        <v>1.500590016828562e-15</v>
       </c>
     </row>
     <row r="93">
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.03366781786149638</v>
+        <v>-7.967749093537576e-10</v>
       </c>
     </row>
     <row r="94">
@@ -1459,7 +1459,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.9579082447707868</v>
+        <v>0.9844814942268494</v>
       </c>
     </row>
     <row r="95">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.005811972108345099</v>
+        <v>-2.12451638785743e-09</v>
       </c>
     </row>
     <row r="96">
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.08716981364432899</v>
+        <v>0.081930321518855</v>
       </c>
     </row>
     <row r="97">
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.04273211332871247</v>
+        <v>-6.267607586438256e-09</v>
       </c>
     </row>
     <row r="98">
@@ -1499,7 +1499,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-1.377200172999205e-13</v>
+        <v>3.22110693120042e-15</v>
       </c>
     </row>
     <row r="99">
@@ -1509,7 +1509,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.005056057548268262</v>
+        <v>-1.649840546740741e-10</v>
       </c>
     </row>
     <row r="100">
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>3.31632488136409</v>
+        <v>2.893252895166951</v>
       </c>
     </row>
     <row r="101">
@@ -1529,7 +1529,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.1537443193982623</v>
+        <v>0.1194706972139097</v>
       </c>
     </row>
     <row r="102">
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.02077408971484931</v>
+        <v>-1.053337804132748e-09</v>
       </c>
     </row>
     <row r="103">
@@ -1549,7 +1549,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.2845493811472461</v>
+        <v>-2.991480078928799e-08</v>
       </c>
     </row>
     <row r="104">
@@ -1559,7 +1559,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.137624663641653</v>
+        <v>0.08204659517439658</v>
       </c>
     </row>
     <row r="105">
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.03366253052316689</v>
+        <v>-4.150885159898143e-09</v>
       </c>
     </row>
     <row r="106">
@@ -1579,7 +1579,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1.861311334618649</v>
+        <v>1.571714374132259</v>
       </c>
     </row>
     <row r="107">
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.7612025616147083</v>
+        <v>0.7730833692395932</v>
       </c>
     </row>
     <row r="108">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.1050273036808776</v>
+        <v>0.1300667733447216</v>
       </c>
     </row>
     <row r="109">
@@ -1609,7 +1609,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.04395720920968223</v>
+        <v>0.009964522977254761</v>
       </c>
     </row>
     <row r="110">
@@ -1629,7 +1629,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-4.336808689942018e-19</v>
+        <v>-1.951563910473908e-18</v>
       </c>
     </row>
     <row r="112">
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.1363602531414446</v>
+        <v>-0.08171383071985455</v>
       </c>
     </row>
     <row r="113">
@@ -1649,7 +1649,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>1.084202172485504e-19</v>
+        <v>-1.592421940838085e-19</v>
       </c>
     </row>
     <row r="114">
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.2518222535968294</v>
+        <v>0.283687908460051</v>
       </c>
     </row>
     <row r="115">
@@ -1689,7 +1689,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.002341440299378448</v>
+        <v>0.002912045769335567</v>
       </c>
     </row>
     <row r="118">
@@ -1699,7 +1699,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-4.335620050715131e-06</v>
+        <v>-5.473122536514518e-09</v>
       </c>
     </row>
     <row r="119">
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-2.05301595839005e-07</v>
+        <v>-3.54018073779551e-10</v>
       </c>
     </row>
     <row r="120">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.0002876031368585023</v>
+        <v>-6.184121745671928e-05</v>
       </c>
     </row>
     <row r="121">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>5.2873383294851e-06</v>
+        <v>3.354110250687772e-09</v>
       </c>
     </row>
     <row r="122">
@@ -1739,7 +1739,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.1247493863506291</v>
+        <v>0.144420588295566</v>
       </c>
     </row>
     <row r="123">
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.001843645627115598</v>
+        <v>0.0009824573252918201</v>
       </c>
     </row>
     <row r="125">
@@ -1769,7 +1769,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.001697073607541842</v>
+        <v>0.001029734088083553</v>
       </c>
     </row>
     <row r="126">
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-1.312436849434648e-20</v>
+        <v>-2.004462042719001e-20</v>
       </c>
     </row>
     <row r="128">
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.0009768073634231172</v>
+        <v>-0.0002709232370838084</v>
       </c>
     </row>
     <row r="129">
@@ -1809,7 +1809,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>9.063882489603044e-21</v>
+        <v>1.585639188626297e-20</v>
       </c>
     </row>
     <row r="130">
@@ -1839,7 +1839,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.2017400425148648</v>
+        <v>0.1333770000485835</v>
       </c>
     </row>
     <row r="133">
@@ -1849,7 +1849,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.1097713618985423</v>
+        <v>0.1183108650794165</v>
       </c>
     </row>
     <row r="134">
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>4.416251575920939</v>
+        <v>5.668814753527495</v>
       </c>
     </row>
     <row r="135">
@@ -1869,7 +1869,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.5410277925926624</v>
+        <v>0.4869366765324509</v>
       </c>
     </row>
     <row r="136">
@@ -1879,7 +1879,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-0.06752736898589817</v>
+        <v>1.72826863030896e-09</v>
       </c>
     </row>
     <row r="137">
@@ -1889,7 +1889,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>-0.5011898217554328</v>
+        <v>3.306101893368849e-08</v>
       </c>
     </row>
     <row r="138">
@@ -1899,7 +1899,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.176650018846517</v>
+        <v>-0.2267525336519681</v>
       </c>
     </row>
     <row r="139">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.06006767655395321</v>
+        <v>-2.499074371224133e-09</v>
       </c>
     </row>
     <row r="140">
@@ -1919,7 +1919,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.05622939444507653</v>
+        <v>0.04289865128533987</v>
       </c>
     </row>
     <row r="141">
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.06750689971058244</v>
+        <v>-6.613047460355122e-06</v>
       </c>
     </row>
     <row r="142">
@@ -1939,7 +1939,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.000106932094702796</v>
+        <v>-1.47418709485834e-07</v>
       </c>
     </row>
     <row r="143">
@@ -1949,7 +1949,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.08165634762443545</v>
+        <v>0.07498834044235578</v>
       </c>
     </row>
     <row r="144">
@@ -1959,7 +1959,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.04062581136348831</v>
+        <v>-0.02499999012464939</v>
       </c>
     </row>
     <row r="145">
@@ -1969,7 +1969,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.01551546059617238</v>
+        <v>7.935290679272146e-07</v>
       </c>
     </row>
     <row r="146">
@@ -1979,7 +1979,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.02045058859542102</v>
+        <v>0.0155638692857712</v>
       </c>
     </row>
     <row r="147">
@@ -1989,7 +1989,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-0.4163952658292929</v>
+        <v>-0.2894543941307604</v>
       </c>
     </row>
     <row r="148">
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.9637254850537458</v>
+        <v>-0.003999685263766927</v>
       </c>
     </row>
     <row r="149">
@@ -2009,7 +2009,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.08358531792353184</v>
+        <v>-0.00216724750756736</v>
       </c>
     </row>
     <row r="150">
@@ -2019,7 +2019,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-0.09898597929354491</v>
+        <v>-0.06588786792411054</v>
       </c>
     </row>
     <row r="151">
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-0.6232751761229282</v>
+        <v>-0.8845379351899274</v>
       </c>
     </row>
     <row r="152">
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.2169140546336944</v>
+        <v>4.34759541575086e-05</v>
       </c>
     </row>
     <row r="153">
@@ -2049,7 +2049,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.1952535059870182</v>
+        <v>-0.2759381839222994</v>
       </c>
     </row>
     <row r="154">
@@ -2059,7 +2059,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.324821065943337</v>
+        <v>0.546945228151907</v>
       </c>
     </row>
     <row r="155">
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>1.350159429070005</v>
+        <v>0.3665173469717813</v>
       </c>
     </row>
     <row r="156">
@@ -2079,7 +2079,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.03966632927836396</v>
+        <v>-1.823992013740275e-09</v>
       </c>
     </row>
     <row r="157">
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.2910838944137767</v>
+        <v>-1.345152199905187e-08</v>
       </c>
     </row>
     <row r="158">
@@ -2099,7 +2099,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-31.3742489021453</v>
+        <v>-14.4710600542043</v>
       </c>
     </row>
     <row r="159">
@@ -2109,7 +2109,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.03431728839391537</v>
+        <v>2.037423588680084e-09</v>
       </c>
     </row>
     <row r="160">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.3139256802699997</v>
+        <v>-1.463320475902918e-05</v>
       </c>
     </row>
     <row r="161">
@@ -2129,7 +2129,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.02791096504151102</v>
+        <v>-1.305286365105296e-06</v>
       </c>
     </row>
     <row r="162">
@@ -2139,7 +2139,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.09802993308310505</v>
+        <v>0.06162873404420342</v>
       </c>
     </row>
     <row r="163">
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.2173620025260267</v>
+        <v>0.1919270248274053</v>
       </c>
     </row>
     <row r="164">
@@ -2159,7 +2159,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.1000115182602959</v>
+        <v>-4.184463572873687e-05</v>
       </c>
     </row>
     <row r="165">
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-0.04114878362914722</v>
+        <v>-0.02541871493359663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>